<commit_message>
Bayesian discrepancy as a vector rather than scalar. Inversion still going. Results to check. Process is extrem. slow
</commit_message>
<xml_diff>
--- a/MRIdata.xlsx
+++ b/MRIdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\IFM\User\melito\Server\Projects\TimeCalibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649D0C62-42CD-456E-885D-86FDE7720F4C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E2BBC6-1D64-459C-8D54-1464C7F39ECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -258,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -307,6 +313,36 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5435,26 +5471,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" style="1"/>
-    <col min="2" max="2" width="11.33203125" style="1"/>
-    <col min="3" max="3" width="19.88671875" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="1"/>
+    <col min="2" max="2" width="11.28515625" style="1"/>
+    <col min="3" max="3" width="19.85546875" style="1"/>
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1"/>
-    <col min="6" max="6" width="10.6640625" style="1"/>
-    <col min="7" max="7" width="8.6640625" style="1"/>
-    <col min="8" max="8" width="10.88671875" style="1"/>
-    <col min="9" max="9" width="8.6640625" style="1"/>
-    <col min="10" max="10" width="10.44140625" style="1"/>
-    <col min="11" max="12" width="8.6640625" style="1"/>
-    <col min="13" max="13" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="1025" width="8.6640625" style="1"/>
-    <col min="1026" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="5" width="20.85546875" style="1"/>
+    <col min="6" max="6" width="10.7109375" style="1"/>
+    <col min="7" max="7" width="8.7109375" style="1"/>
+    <col min="8" max="8" width="10.85546875" style="1"/>
+    <col min="9" max="9" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="10.42578125" style="1"/>
+    <col min="11" max="12" width="8.7109375" style="1"/>
+    <col min="13" max="13" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="1025" width="8.7109375" style="1"/>
+    <col min="1026" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
@@ -5942,244 +5978,244 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1">
-      <c r="A20" s="15"/>
-      <c r="B20" s="3">
+      <c r="A20" s="21"/>
+      <c r="B20" s="22">
         <v>0</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="22">
         <v>0</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="22">
         <v>0</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="22">
         <v>0</v>
       </c>
-      <c r="F20" s="3">
+      <c r="F20" s="22">
         <v>0</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="22">
         <v>0</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="22">
         <v>0</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="22">
         <v>0</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="23">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="15"/>
-      <c r="B21" s="3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22">
         <v>5</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="22">
         <v>2.6298583833333299E-2</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="22">
         <v>3.3409184057535701E-3</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="22">
         <v>0.27709552999999998</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="22">
         <v>2.4227987527914802E-2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="22">
         <v>0.92228228228228204</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="22">
         <v>4.3359470098824501E-2</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="22">
         <v>1.99626666666667</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="23">
         <v>0.18301821160140799</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="15"/>
-      <c r="B22" s="3">
+      <c r="A22" s="21"/>
+      <c r="B22" s="22">
         <v>10</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="22">
         <v>4.5606605666666702E-2</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="22">
         <v>6.6291773597904804E-3</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="22">
         <v>0.44065893833333297</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="22">
         <v>4.8805595324181099E-2</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G22" s="22">
         <v>0.95363363363363396</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="22">
         <v>5.30616949540752E-2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="22">
         <v>3.2933333333333299</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="23">
         <v>0.33353909382726199</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="15"/>
-      <c r="B23" s="3">
+      <c r="A23" s="21"/>
+      <c r="B23" s="22">
         <v>15</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="22">
         <v>6.4312643833333294E-2</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="22">
         <v>8.6441531896319906E-3</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="22">
         <v>0.59811692500000002</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F23" s="22">
         <v>4.3798455017492202E-2</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G23" s="22">
         <v>0.93765765765765796</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="22">
         <v>3.9094698137336702E-2</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="22">
         <v>4.6410666666666698</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="23">
         <v>0.217052120724749</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="15"/>
-      <c r="B24" s="3">
+      <c r="A24" s="21"/>
+      <c r="B24" s="22">
         <v>20</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="22">
         <v>7.2278479500000006E-2</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="22">
         <v>4.8392209171200604E-3</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="22">
         <v>0.67791570000000001</v>
       </c>
-      <c r="F24" s="3">
+      <c r="F24" s="22">
         <v>3.6460494595429702E-2</v>
       </c>
-      <c r="G24" s="3">
+      <c r="G24" s="22">
         <v>0.92672672672672696</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="22">
         <v>4.9883182893026602E-2</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="22">
         <v>5.1781333333333297</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="23">
         <v>0.15770279783328001</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="15"/>
-      <c r="B25" s="3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="22">
         <v>25</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="22">
         <v>6.7903108333333295E-2</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="22">
         <v>4.5097320964668499E-3</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="22">
         <v>0.65796358333333305</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="22">
         <v>3.5398342629814901E-2</v>
       </c>
-      <c r="G25" s="3">
+      <c r="G25" s="22">
         <v>0.90882882882882898</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="22">
         <v>3.9595935503264103E-2</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="22">
         <v>5.1832000000000003</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="23">
         <v>0.194615408776729</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="16"/>
-      <c r="B26" s="7">
+      <c r="A26" s="24"/>
+      <c r="B26" s="25">
         <v>30</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="25">
         <v>6.9270807166666698E-2</v>
       </c>
-      <c r="D26" s="7">
+      <c r="D26" s="25">
         <v>4.2817183710424003E-3</v>
       </c>
-      <c r="E26" s="7">
+      <c r="E26" s="25">
         <v>0.66988936666666699</v>
       </c>
-      <c r="F26" s="7">
+      <c r="F26" s="25">
         <v>3.28814542304438E-2</v>
       </c>
-      <c r="G26" s="7">
+      <c r="G26" s="25">
         <v>0.92180180180180205</v>
       </c>
-      <c r="H26" s="7">
+      <c r="H26" s="25">
         <v>3.5480157049355802E-2</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="25">
         <v>5.3098666666666698</v>
       </c>
-      <c r="J26" s="10">
+      <c r="J26" s="26">
         <v>0.229604428915859</v>
       </c>
     </row>
@@ -6217,7 +6253,7 @@
     </row>
     <row r="29" spans="1:10">
       <c r="D29" s="1">
-        <f t="shared" ref="D29:F35" si="0">D21^2</f>
+        <f t="shared" ref="D29:F34" si="0">D21^2</f>
         <v>1.1161735793902976E-5</v>
       </c>
       <c r="F29" s="1">

</xml_diff>

<commit_message>
Discrepancy module seems to have problems. Restore to main branch due to inversion problems
</commit_message>
<xml_diff>
--- a/MRIdata.xlsx
+++ b/MRIdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\IFM\User\melito\Server\Projects\TimeCalibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E2BBC6-1D64-459C-8D54-1464C7F39ECE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADC1585A-4464-4FBD-8223-D18D76F40B5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="996" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -305,6 +305,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -317,32 +338,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5494,7 +5494,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="2" customFormat="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="21" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -5526,7 +5526,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1">
-      <c r="A2" s="15"/>
+      <c r="A2" s="22"/>
       <c r="B2" s="3">
         <v>0</v>
       </c>
@@ -5556,7 +5556,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="15"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="3">
         <v>5</v>
       </c>
@@ -5586,7 +5586,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="15"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="3">
         <v>10</v>
       </c>
@@ -5616,7 +5616,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="15"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="3">
         <v>15</v>
       </c>
@@ -5646,7 +5646,7 @@
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="15"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="3">
         <v>20</v>
       </c>
@@ -5676,7 +5676,7 @@
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="15"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="3">
         <v>25</v>
       </c>
@@ -5706,7 +5706,7 @@
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="16"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="7">
         <v>30</v>
       </c>
@@ -5736,7 +5736,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -5768,7 +5768,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1">
-      <c r="A11" s="15"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="3">
         <v>0</v>
       </c>
@@ -5798,7 +5798,7 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="15"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="3">
         <v>5</v>
       </c>
@@ -5828,7 +5828,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="15"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="3">
         <v>10</v>
       </c>
@@ -5858,7 +5858,7 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="15"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="3">
         <v>15</v>
       </c>
@@ -5888,7 +5888,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="15"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="3">
         <v>20</v>
       </c>
@@ -5918,7 +5918,7 @@
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="15"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="3">
         <v>25</v>
       </c>
@@ -5948,7 +5948,7 @@
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="16"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="7">
         <v>30</v>
       </c>
@@ -5978,244 +5978,244 @@
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22">
+      <c r="A20" s="25"/>
+      <c r="B20" s="17">
         <v>0</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="17">
         <v>0</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="17">
         <v>0</v>
       </c>
-      <c r="E20" s="22">
+      <c r="E20" s="17">
         <v>0</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="17">
         <v>0</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="17">
         <v>0</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="17">
         <v>0</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="17">
         <v>0</v>
       </c>
-      <c r="J20" s="23">
+      <c r="J20" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22">
+      <c r="A21" s="25"/>
+      <c r="B21" s="17">
         <v>5</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="17">
         <v>2.6298583833333299E-2</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="17">
         <v>3.3409184057535701E-3</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E21" s="17">
         <v>0.27709552999999998</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="17">
         <v>2.4227987527914802E-2</v>
       </c>
-      <c r="G21" s="22">
+      <c r="G21" s="17">
         <v>0.92228228228228204</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="17">
         <v>4.3359470098824501E-2</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="17">
         <v>1.99626666666667</v>
       </c>
-      <c r="J21" s="23">
+      <c r="J21" s="18">
         <v>0.18301821160140799</v>
       </c>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22">
+      <c r="A22" s="25"/>
+      <c r="B22" s="17">
         <v>10</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="17">
         <v>4.5606605666666702E-2</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="17">
         <v>6.6291773597904804E-3</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="17">
         <v>0.44065893833333297</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="17">
         <v>4.8805595324181099E-2</v>
       </c>
-      <c r="G22" s="22">
+      <c r="G22" s="17">
         <v>0.95363363363363396</v>
       </c>
-      <c r="H22" s="22">
+      <c r="H22" s="17">
         <v>5.30616949540752E-2</v>
       </c>
-      <c r="I22" s="22">
+      <c r="I22" s="17">
         <v>3.2933333333333299</v>
       </c>
-      <c r="J22" s="23">
+      <c r="J22" s="18">
         <v>0.33353909382726199</v>
       </c>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22">
+      <c r="A23" s="25"/>
+      <c r="B23" s="17">
         <v>15</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="17">
         <v>6.4312643833333294E-2</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="17">
         <v>8.6441531896319906E-3</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="17">
         <v>0.59811692500000002</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="17">
         <v>4.3798455017492202E-2</v>
       </c>
-      <c r="G23" s="22">
+      <c r="G23" s="17">
         <v>0.93765765765765796</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="17">
         <v>3.9094698137336702E-2</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="17">
         <v>4.6410666666666698</v>
       </c>
-      <c r="J23" s="23">
+      <c r="J23" s="18">
         <v>0.217052120724749</v>
       </c>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="21"/>
-      <c r="B24" s="22">
+      <c r="A24" s="25"/>
+      <c r="B24" s="17">
         <v>20</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="17">
         <v>7.2278479500000006E-2</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="17">
         <v>4.8392209171200604E-3</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="17">
         <v>0.67791570000000001</v>
       </c>
-      <c r="F24" s="22">
+      <c r="F24" s="17">
         <v>3.6460494595429702E-2</v>
       </c>
-      <c r="G24" s="22">
+      <c r="G24" s="17">
         <v>0.92672672672672696</v>
       </c>
-      <c r="H24" s="22">
+      <c r="H24" s="17">
         <v>4.9883182893026602E-2</v>
       </c>
-      <c r="I24" s="22">
+      <c r="I24" s="17">
         <v>5.1781333333333297</v>
       </c>
-      <c r="J24" s="23">
+      <c r="J24" s="18">
         <v>0.15770279783328001</v>
       </c>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="21"/>
-      <c r="B25" s="22">
+      <c r="A25" s="25"/>
+      <c r="B25" s="17">
         <v>25</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="17">
         <v>6.7903108333333295E-2</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="17">
         <v>4.5097320964668499E-3</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="17">
         <v>0.65796358333333305</v>
       </c>
-      <c r="F25" s="22">
+      <c r="F25" s="17">
         <v>3.5398342629814901E-2</v>
       </c>
-      <c r="G25" s="22">
+      <c r="G25" s="17">
         <v>0.90882882882882898</v>
       </c>
-      <c r="H25" s="22">
+      <c r="H25" s="17">
         <v>3.9595935503264103E-2</v>
       </c>
-      <c r="I25" s="22">
+      <c r="I25" s="17">
         <v>5.1832000000000003</v>
       </c>
-      <c r="J25" s="23">
+      <c r="J25" s="18">
         <v>0.194615408776729</v>
       </c>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="19">
         <v>30</v>
       </c>
-      <c r="C26" s="25">
+      <c r="C26" s="19">
         <v>6.9270807166666698E-2</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="19">
         <v>4.2817183710424003E-3</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="19">
         <v>0.66988936666666699</v>
       </c>
-      <c r="F26" s="25">
+      <c r="F26" s="19">
         <v>3.28814542304438E-2</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="19">
         <v>0.92180180180180205</v>
       </c>
-      <c r="H26" s="25">
+      <c r="H26" s="19">
         <v>3.5480157049355802E-2</v>
       </c>
-      <c r="I26" s="25">
+      <c r="I26" s="19">
         <v>5.3098666666666698</v>
       </c>
-      <c r="J26" s="26">
+      <c r="J26" s="20">
         <v>0.229604428915859</v>
       </c>
     </row>

</xml_diff>